<commit_message>
updates to filtering. switched from groupfilter to index filter in the cc_plotter function because it was causing errors when running in JupyterHub test environment ahead of workshop.
</commit_message>
<xml_diff>
--- a/Sample_Data/ccs_2DOC_CAMELS_1_S_True_60_60_TEVA007.xlsx
+++ b/Sample_Data/ccs_2DOC_CAMELS_1_S_True_60_60_TEVA007.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uvmoffice-my.sharepoint.com/personal/rvanderh_uvm_edu/Documents/Documents/_UVM/Research/CIROH/TEVA/TEVA_Post_Processing/Sample_Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="11_2B770FFFEED41C5ACB3B3495395BDA1666CE9269" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5B8B327F-5C7B-4541-ADA8-7A7A56DA0AF9}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="11_2B770FFFEED41C5ACB3B3495395BDA1666CE9269" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CF4DD50F-CDBA-B94B-A076-69CC389E2765}"/>
   <bookViews>
-    <workbookView xWindow="160" yWindow="1040" windowWidth="35680" windowHeight="22180" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="160" yWindow="660" windowWidth="68480" windowHeight="27980" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CCEA_High" sheetId="1" r:id="rId1"/>
@@ -1111,10 +1111,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5827,11 +5823,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:BT83"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P5" sqref="P5"/>
+    <sheetView tabSelected="1" zoomScale="152" zoomScaleNormal="152" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="9" max="9" width="16.83203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="17.1640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:72" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">

</xml_diff>